<commit_message>
fuck need to calibrate neutral points seperately for tof and camera
</commit_message>
<xml_diff>
--- a/pixel_to_cm.xlsx
+++ b/pixel_to_cm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtanh\Documents\thiccWIRES-2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D933811-3483-4ECD-B896-BC1AA6DB9860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B60B82D-BF68-4DCA-BA5C-D4200B70C453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{D76589F0-36FB-4250-B5EF-676EB3C29F02}"/>
   </bookViews>
@@ -392,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8040B9C9-F767-48AB-A2D1-2ADF42158E32}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+      <selection activeCell="B53" sqref="A1:B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -410,31 +410,418 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B2">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B3">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>25</v>
+      </c>
+      <c r="B22">
+        <v>103.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>30</v>
+      </c>
+      <c r="B23">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>35</v>
+      </c>
+      <c r="B24">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>40</v>
+      </c>
+      <c r="B25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>45</v>
+      </c>
+      <c r="B26">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>50</v>
+      </c>
+      <c r="B27">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>55</v>
+      </c>
+      <c r="B28">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>60</v>
+      </c>
+      <c r="B29">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>65</v>
+      </c>
+      <c r="B30">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>70</v>
+      </c>
+      <c r="B31">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>75</v>
+      </c>
+      <c r="B32">
+        <v>133.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>80</v>
+      </c>
+      <c r="B33">
+        <v>134.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>85</v>
+      </c>
+      <c r="B34">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>90</v>
+      </c>
+      <c r="B35">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>95</v>
+      </c>
+      <c r="B36">
+        <v>137.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>100</v>
+      </c>
+      <c r="B37">
+        <v>138.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>105</v>
+      </c>
+      <c r="B38">
+        <v>139.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>110</v>
+      </c>
+      <c r="B39">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>115</v>
+      </c>
+      <c r="B40">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>120</v>
+      </c>
+      <c r="B41">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>125</v>
+      </c>
+      <c r="B42">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>130</v>
+      </c>
+      <c r="B43">
+        <v>141.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>135</v>
+      </c>
+      <c r="B44">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>140</v>
+      </c>
+      <c r="B45">
+        <v>142.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>145</v>
+      </c>
+      <c r="B46">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>150</v>
+      </c>
+      <c r="B47">
+        <v>143.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>155</v>
+      </c>
+      <c r="B48">
+        <v>143.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>160</v>
+      </c>
+      <c r="B49">
+        <v>144.5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>165</v>
+      </c>
+      <c r="B50">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>170</v>
+      </c>
+      <c r="B51">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>175</v>
+      </c>
+      <c r="B52">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>180</v>
+      </c>
+      <c r="B53">
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>